<commit_message>
Changed Video file to include price
</commit_message>
<xml_diff>
--- a/Venky-Submission Sheet- Innovation Track.xlsx
+++ b/Venky-Submission Sheet- Innovation Track.xlsx
@@ -115,75 +115,21 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Humbhi online has these functionalities in the application. The application is open sourced. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/venkatramanm/humbhionline
+    <t xml:space="preserve">Humbhi online has these functionalities in the application. The application is open sourced. https://github.com/venkatramanm/humbhionline
 Any user can be a seller.
 User can define his/her upi handle.
 Seller can define facilities/stores
 Items stocked in stores can be added to the store’s catalog (* Open catalog dataset project will help adding it quicker *)
 Item details can be added for sellers.
-Store can mention if it supports delivery or buyer needs to pickup . Store can outsource delivery via 3</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">rd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve"> party (Dunzo good box etc. Humbhionline is a delivery BAP)</t>
-    </r>
+Store can mention if it supports delivery or buyer needs to pickup . Store can outsource delivery via 3rd party (Dunzo good box etc. Humbhionline is a delivery BAP)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Loaded the XLS provided in the hackathon and made it available to sellers on humbhionline
+    <t xml:space="preserve">Loaded the XLS provided in the hackathon and made it available to sellers on humbhionline
 https://mandi.succinct.in  is a the stage instance of the opensource project https://github.com/venkatramanm/humbhionline 
 The production instance is https://humbhionline.in  where it will be made available shortly
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A POC Client app has been written which can be seen for the implementation of this open catalog VID_20220109_105520_257.mp4 
-https://github.com/venkatramanm/innovation-hackathon-jan22/blob/main/VID_20220109_105520_257.mp4</t>
-    </r>
+A POC Client app has been written which can be seen for the implementation of this open catalog.
+prototype-video.mp4
+https://github.com/venkatramanm/innovation-hackathon-jan22/blob/main/prototype-video.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">Regular Flutter Application
@@ -197,42 +143,13 @@
     <t xml:space="preserve">b</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Open FMCG DataSet Api
+    <t xml:space="preserve">Open FMCG DataSet Api
 Catalog Text Search 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">curl -H "Accept:application/json" https://mandi.succinct.in/skus/open_search?q=Maggi
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lato"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
+curl -H "Accept:application/json" https://mandi.succinct.in/skus/open_search?q=Maggi
 Catalog OCR Search provided
 curl -H "Accept:application/json" -F file=@database/images/Maggi_2_Minute_Noodels.png  https://mandi.succinct.in/skus/image_search 
  ** Prototype added for this Part* 
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Dataset made available in the hackathon by Supriyo and Good box team were used</t>
@@ -329,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -414,19 +331,6 @@
       <name val="Lato"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Lato"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Lato"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -632,7 +536,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -718,10 +622,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -848,21 +748,21 @@
   </sheetPr>
   <dimension ref="A1:AG1033"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="65.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="10" style="1" width="19.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1170,7 +1070,7 @@
       <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>25</v>
       </c>
       <c r="I8" s="21" t="s">
@@ -1219,8 +1119,8 @@
       <c r="G9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="21" t="s">
         <v>30</v>
       </c>
@@ -1260,8 +1160,8 @@
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
@@ -1303,8 +1203,8 @@
       <c r="G11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="21"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
@@ -1342,8 +1242,8 @@
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="21"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
@@ -1381,8 +1281,8 @@
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="21"/>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
@@ -1420,8 +1320,8 @@
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
@@ -37464,7 +37364,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G8" r:id="rId1" display="https://github.com/venkatramanm/humbhionline"/>
+    <hyperlink ref="G8" r:id="rId1" display="Humbhi online has these functionalities in the application. The application is open sourced. https://github.com/venkatramanm/humbhionline&#10;&#10;Any user can be a seller.&#10;User can define his/her upi handle.&#10;Seller can define facilities/stores&#10;Items stocked in stores can be added to the store’s catalog (* Open catalog dataset project will help adding it quicker *)&#10;Item details can be added for sellers.&#10;Store can mention if it supports delivery or buyer needs to pickup . Store can outsource delivery via 3rd party (Dunzo good box etc. Humbhionline is a delivery BAP)"/>
+    <hyperlink ref="H8" r:id="rId2" display="https://github.com/venkatramanm/innovation-hackathon-jan22/blob/main/prototype-video.mp4"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Moved othr artificats to google docs
</commit_message>
<xml_diff>
--- a/Venky-Submission Sheet- Innovation Track.xlsx
+++ b/Venky-Submission Sheet- Innovation Track.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="58">
   <si>
     <r>
       <rPr>
@@ -128,8 +128,10 @@
 https://mandi.succinct.in  is a the stage instance of the opensource project https://github.com/venkatramanm/humbhionline 
 The production instance is https://humbhionline.in  where it will be made available shortly
 A POC Client app has been written which can be seen for the implementation of this open catalog.
-prototype-video.mp4
-https://github.com/venkatramanm/innovation-hackathon-jan22/blob/main/prototype-video.mp4</t>
+(Video)
+https://drive.google.com/file/d/1GYAcgEGH1NaisKR7hFDmOuqs-s-8Y0PL/view?usp=sharing, 
+(Screen Shot of seller with 1000+  items Loaded)
+https://drive.google.com/file/d/1HGRIJ2_zTiTs7zBgtkEroo7c_ISp9KXj/view?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">Regular Flutter Application
@@ -193,9 +195,6 @@
   </si>
   <si>
     <t xml:space="preserve">Enable intelligent searches, for different buyer apps in the ONDC network, so that there is better discoverability of seller catalogs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">curl -H "Accept:application/json" -F file=@database/images/Maggi_2_Minute_Noodels.png  https://mandi.succinct.in/skus/image_search</t>
   </si>
   <si>
     <t xml:space="preserve">Dynamic Pricing</t>
@@ -749,8 +748,8 @@
   </sheetPr>
   <dimension ref="A1:AG1033"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -759,8 +758,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="65.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="55.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="45.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="28.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="10" style="1" width="19.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="15" style="1" width="14.43"/>
@@ -1861,7 +1860,7 @@
       <c r="AF27" s="14"/>
       <c r="AG27" s="14"/>
     </row>
-    <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1872,9 +1871,7 @@
         <v>35</v>
       </c>
       <c r="F28" s="21"/>
-      <c r="G28" s="21" t="s">
-        <v>44</v>
-      </c>
+      <c r="G28" s="0"/>
       <c r="H28" s="21"/>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
@@ -1942,10 +1939,10 @@
         <v>5</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="14" t="s">
         <v>21</v>
@@ -2139,10 +2136,10 @@
         <v>6</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>21</v>
@@ -2336,10 +2333,10 @@
         <v>7</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>21</v>
@@ -2533,10 +2530,10 @@
         <v>8</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>21</v>
@@ -2691,10 +2688,10 @@
         <v>9</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D49" s="14" t="s">
         <v>21</v>
@@ -2888,10 +2885,10 @@
         <v>10</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>21</v>
@@ -3085,10 +3082,10 @@
         <v>11</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="14" t="s">
         <v>21</v>

</xml_diff>